<commit_message>
Modificación de los nombres de las tablas y de algunos atributos
</commit_message>
<xml_diff>
--- a/alimentos cárnicos - data.xlsx
+++ b/alimentos cárnicos - data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documentos\GitHub\prueba técnica alimentos cárnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F1674E-17C3-40E8-AF62-36AAD65DC0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0F76CF-8070-4654-90C0-262D5BB1F479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7967CFBD-3329-4BA7-A577-6C1F0DD0E57F}"/>
   </bookViews>
@@ -182,12 +182,6 @@
     <t>Fecha_compra</t>
   </si>
   <si>
-    <t>Clientes Data</t>
-  </si>
-  <si>
-    <t>Compras Data</t>
-  </si>
-  <si>
     <t>Tocinetas Ahumadas 200 g</t>
   </si>
   <si>
@@ -233,7 +227,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Precio c/u</t>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Precio_unitario</t>
   </si>
 </sst>
 </file>
@@ -533,6 +533,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,15 +550,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E85538-3410-4A03-AD45-0DFA31173A94}">
   <dimension ref="B1:T53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,7 +900,7 @@
     <col min="7" max="7" width="10.109375" customWidth="1"/>
     <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -909,21 +909,21 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="G2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="20"/>
+      <c r="B2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="G2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="23"/>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
@@ -954,7 +954,7 @@
         <v>46</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>47</v>
@@ -980,9 +980,9 @@
         <v>1</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="21">
+        <v>48</v>
+      </c>
+      <c r="J4" s="18">
         <v>13050</v>
       </c>
       <c r="K4" s="9">
@@ -1016,9 +1016,9 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="22">
+        <v>49</v>
+      </c>
+      <c r="J5" s="19">
         <v>11900</v>
       </c>
       <c r="K5" s="2">
@@ -1052,9 +1052,9 @@
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="22">
+        <v>50</v>
+      </c>
+      <c r="J6" s="19">
         <v>13048</v>
       </c>
       <c r="K6" s="2">
@@ -1088,9 +1088,9 @@
         <v>2</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="22">
+        <v>51</v>
+      </c>
+      <c r="J7" s="19">
         <v>5350</v>
       </c>
       <c r="K7" s="2">
@@ -1124,9 +1124,9 @@
         <v>3</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="22">
+        <v>52</v>
+      </c>
+      <c r="J8" s="19">
         <v>25990</v>
       </c>
       <c r="K8" s="2">
@@ -1160,9 +1160,9 @@
         <v>3</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="22">
+        <v>53</v>
+      </c>
+      <c r="J9" s="19">
         <v>3890</v>
       </c>
       <c r="K9" s="2">
@@ -1196,9 +1196,9 @@
         <v>4</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="22">
+        <v>54</v>
+      </c>
+      <c r="J10" s="19">
         <v>15850</v>
       </c>
       <c r="K10" s="2">
@@ -1238,9 +1238,9 @@
         <v>4</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="22">
+        <v>55</v>
+      </c>
+      <c r="J11" s="19">
         <v>13390</v>
       </c>
       <c r="K11" s="2">
@@ -1274,9 +1274,9 @@
         <v>5</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="22">
+        <v>56</v>
+      </c>
+      <c r="J12" s="19">
         <v>11040</v>
       </c>
       <c r="K12" s="2">
@@ -1310,9 +1310,9 @@
         <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="22">
+        <v>57</v>
+      </c>
+      <c r="J13" s="19">
         <v>5944</v>
       </c>
       <c r="K13" s="2">
@@ -1346,9 +1346,9 @@
         <v>6</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="22">
+        <v>58</v>
+      </c>
+      <c r="J14" s="19">
         <v>7950</v>
       </c>
       <c r="K14" s="2">
@@ -1382,9 +1382,9 @@
         <v>6</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="22">
+        <v>48</v>
+      </c>
+      <c r="J15" s="19">
         <v>13050</v>
       </c>
       <c r="K15" s="2">
@@ -1418,9 +1418,9 @@
         <v>7</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="22">
+        <v>49</v>
+      </c>
+      <c r="J16" s="19">
         <v>11900</v>
       </c>
       <c r="K16" s="2">
@@ -1454,9 +1454,9 @@
         <v>7</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="22">
+        <v>50</v>
+      </c>
+      <c r="J17" s="19">
         <v>13048</v>
       </c>
       <c r="K17" s="2">
@@ -1490,9 +1490,9 @@
         <v>8</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="22">
+        <v>51</v>
+      </c>
+      <c r="J18" s="19">
         <v>5350</v>
       </c>
       <c r="K18" s="2">
@@ -1526,9 +1526,9 @@
         <v>8</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J19" s="22">
+        <v>52</v>
+      </c>
+      <c r="J19" s="19">
         <v>25990</v>
       </c>
       <c r="K19" s="2">
@@ -1562,9 +1562,9 @@
         <v>9</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J20" s="22">
+        <v>53</v>
+      </c>
+      <c r="J20" s="19">
         <v>3890</v>
       </c>
       <c r="K20" s="2">
@@ -1598,9 +1598,9 @@
         <v>9</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="22">
+        <v>54</v>
+      </c>
+      <c r="J21" s="19">
         <v>15850</v>
       </c>
       <c r="K21" s="2">
@@ -1634,9 +1634,9 @@
         <v>10</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" s="22">
+        <v>55</v>
+      </c>
+      <c r="J22" s="19">
         <v>13390</v>
       </c>
       <c r="K22" s="2">
@@ -1670,9 +1670,9 @@
         <v>10</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J23" s="22">
+        <v>56</v>
+      </c>
+      <c r="J23" s="19">
         <v>11040</v>
       </c>
       <c r="K23" s="2">
@@ -1694,9 +1694,9 @@
         <v>11</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J24" s="22">
+        <v>57</v>
+      </c>
+      <c r="J24" s="19">
         <v>5944</v>
       </c>
       <c r="K24" s="2">
@@ -1718,9 +1718,9 @@
         <v>11</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25" s="22">
+        <v>58</v>
+      </c>
+      <c r="J25" s="19">
         <v>7950</v>
       </c>
       <c r="K25" s="2">
@@ -1742,9 +1742,9 @@
         <v>12</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="22">
+        <v>48</v>
+      </c>
+      <c r="J26" s="19">
         <v>13050</v>
       </c>
       <c r="K26" s="2">
@@ -1766,9 +1766,9 @@
         <v>12</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="22">
+        <v>49</v>
+      </c>
+      <c r="J27" s="19">
         <v>11900</v>
       </c>
       <c r="K27" s="2">
@@ -1790,9 +1790,9 @@
         <v>13</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J28" s="22">
+        <v>50</v>
+      </c>
+      <c r="J28" s="19">
         <v>13048</v>
       </c>
       <c r="K28" s="2">
@@ -1814,9 +1814,9 @@
         <v>13</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="22">
+        <v>51</v>
+      </c>
+      <c r="J29" s="19">
         <v>5350</v>
       </c>
       <c r="K29" s="2">
@@ -1838,9 +1838,9 @@
         <v>14</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="22">
+        <v>52</v>
+      </c>
+      <c r="J30" s="19">
         <v>25990</v>
       </c>
       <c r="K30" s="2">
@@ -1862,9 +1862,9 @@
         <v>14</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J31" s="22">
+        <v>53</v>
+      </c>
+      <c r="J31" s="19">
         <v>3890</v>
       </c>
       <c r="K31" s="2">
@@ -1886,9 +1886,9 @@
         <v>15</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J32" s="22">
+        <v>54</v>
+      </c>
+      <c r="J32" s="19">
         <v>15850</v>
       </c>
       <c r="K32" s="2">
@@ -1910,9 +1910,9 @@
         <v>15</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="22">
+        <v>55</v>
+      </c>
+      <c r="J33" s="19">
         <v>13390</v>
       </c>
       <c r="K33" s="2">
@@ -1934,9 +1934,9 @@
         <v>16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J34" s="22">
+        <v>56</v>
+      </c>
+      <c r="J34" s="19">
         <v>11040</v>
       </c>
       <c r="K34" s="2">
@@ -1958,9 +1958,9 @@
         <v>16</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J35" s="22">
+        <v>57</v>
+      </c>
+      <c r="J35" s="19">
         <v>5944</v>
       </c>
       <c r="K35" s="2">
@@ -1982,9 +1982,9 @@
         <v>17</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J36" s="22">
+        <v>58</v>
+      </c>
+      <c r="J36" s="19">
         <v>7950</v>
       </c>
       <c r="K36" s="2">
@@ -2006,9 +2006,9 @@
         <v>17</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J37" s="22">
+        <v>48</v>
+      </c>
+      <c r="J37" s="19">
         <v>13050</v>
       </c>
       <c r="K37" s="2">
@@ -2030,9 +2030,9 @@
         <v>18</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J38" s="22">
+        <v>49</v>
+      </c>
+      <c r="J38" s="19">
         <v>11900</v>
       </c>
       <c r="K38" s="2">
@@ -2054,9 +2054,9 @@
         <v>18</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J39" s="22">
+        <v>50</v>
+      </c>
+      <c r="J39" s="19">
         <v>13048</v>
       </c>
       <c r="K39" s="2">
@@ -2078,9 +2078,9 @@
         <v>19</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J40" s="22">
+        <v>51</v>
+      </c>
+      <c r="J40" s="19">
         <v>5350</v>
       </c>
       <c r="K40" s="2">
@@ -2102,9 +2102,9 @@
         <v>19</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J41" s="22">
+        <v>52</v>
+      </c>
+      <c r="J41" s="19">
         <v>25990</v>
       </c>
       <c r="K41" s="2">
@@ -2126,9 +2126,9 @@
         <v>20</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J42" s="22">
+        <v>59</v>
+      </c>
+      <c r="J42" s="19">
         <v>3890</v>
       </c>
       <c r="K42" s="2">
@@ -2150,9 +2150,9 @@
         <v>20</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J43" s="22">
+        <v>54</v>
+      </c>
+      <c r="J43" s="19">
         <v>15850</v>
       </c>
       <c r="K43" s="2">
@@ -2174,9 +2174,9 @@
         <v>1</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J44" s="22">
+        <v>55</v>
+      </c>
+      <c r="J44" s="19">
         <v>13390</v>
       </c>
       <c r="K44" s="2">
@@ -2198,9 +2198,9 @@
         <v>2</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J45" s="22">
+        <v>56</v>
+      </c>
+      <c r="J45" s="19">
         <v>11040</v>
       </c>
       <c r="K45" s="2">
@@ -2222,9 +2222,9 @@
         <v>3</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J46" s="22">
+        <v>57</v>
+      </c>
+      <c r="J46" s="19">
         <v>5944</v>
       </c>
       <c r="K46" s="2">
@@ -2246,9 +2246,9 @@
         <v>4</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J47" s="22">
+        <v>58</v>
+      </c>
+      <c r="J47" s="19">
         <v>7950</v>
       </c>
       <c r="K47" s="2">
@@ -2270,9 +2270,9 @@
         <v>5</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J48" s="22">
+        <v>48</v>
+      </c>
+      <c r="J48" s="19">
         <v>13050</v>
       </c>
       <c r="K48" s="2">
@@ -2294,9 +2294,9 @@
         <v>6</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J49" s="22">
+        <v>49</v>
+      </c>
+      <c r="J49" s="19">
         <v>11900</v>
       </c>
       <c r="K49" s="2">
@@ -2318,9 +2318,9 @@
         <v>7</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J50" s="22">
+        <v>50</v>
+      </c>
+      <c r="J50" s="19">
         <v>13048</v>
       </c>
       <c r="K50" s="2">
@@ -2342,9 +2342,9 @@
         <v>8</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J51" s="22">
+        <v>60</v>
+      </c>
+      <c r="J51" s="19">
         <v>5350</v>
       </c>
       <c r="K51" s="2">
@@ -2366,9 +2366,9 @@
         <v>9</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J52" s="22">
+        <v>52</v>
+      </c>
+      <c r="J52" s="19">
         <v>25990</v>
       </c>
       <c r="K52" s="2">
@@ -2390,9 +2390,9 @@
         <v>10</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J53" s="23">
+        <v>61</v>
+      </c>
+      <c r="J53" s="20">
         <v>3890</v>
       </c>
       <c r="K53" s="6">

</xml_diff>

<commit_message>
Se módifico la base de datos para usar cédulas en el cliente_id
</commit_message>
<xml_diff>
--- a/alimentos cárnicos - data.xlsx
+++ b/alimentos cárnicos - data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documentos\GitHub\prueba técnica alimentos cárnicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0F76CF-8070-4654-90C0-262D5BB1F479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B5CD2-20F4-4FCA-8B19-23B5CA14112D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7967CFBD-3329-4BA7-A577-6C1F0DD0E57F}"/>
   </bookViews>
@@ -888,7 +888,7 @@
   <dimension ref="B1:T53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,7 +898,7 @@
     <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -962,7 +962,7 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
-        <v>1</v>
+        <v>1045012301</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>4</v>
@@ -976,8 +976,8 @@
       <c r="G4" s="8">
         <v>1</v>
       </c>
-      <c r="H4" s="9">
-        <v>1</v>
+      <c r="H4" s="8">
+        <v>1045012301</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>48</v>
@@ -997,8 +997,8 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
-        <v>2</v>
+      <c r="B5" s="8">
+        <v>1045012302</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1012,8 +1012,8 @@
       <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
+      <c r="H5" s="8">
+        <v>1045012301</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>49</v>
@@ -1033,8 +1033,8 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
-        <v>3</v>
+      <c r="B6" s="8">
+        <v>1045012303</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -1048,8 +1048,8 @@
       <c r="G6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="2">
-        <v>2</v>
+      <c r="H6" s="8">
+        <v>1045012302</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>50</v>
@@ -1069,8 +1069,8 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
-        <v>4</v>
+      <c r="B7" s="8">
+        <v>1045012304</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -1084,8 +1084,8 @@
       <c r="G7" s="3">
         <v>4</v>
       </c>
-      <c r="H7" s="2">
-        <v>2</v>
+      <c r="H7" s="8">
+        <v>1045012302</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>51</v>
@@ -1105,8 +1105,8 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
-        <v>5</v>
+      <c r="B8" s="8">
+        <v>1045012305</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -1120,8 +1120,8 @@
       <c r="G8" s="3">
         <v>5</v>
       </c>
-      <c r="H8" s="2">
-        <v>3</v>
+      <c r="H8" s="8">
+        <v>1045012303</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>52</v>
@@ -1141,8 +1141,8 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
-        <v>6</v>
+      <c r="B9" s="8">
+        <v>1045012306</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -1156,8 +1156,8 @@
       <c r="G9" s="3">
         <v>6</v>
       </c>
-      <c r="H9" s="2">
-        <v>3</v>
+      <c r="H9" s="8">
+        <v>1045012303</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>53</v>
@@ -1177,8 +1177,8 @@
       </c>
     </row>
     <row r="10" spans="2:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
-        <v>7</v>
+      <c r="B10" s="8">
+        <v>1045012307</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1192,8 +1192,8 @@
       <c r="G10" s="3">
         <v>7</v>
       </c>
-      <c r="H10" s="2">
-        <v>4</v>
+      <c r="H10" s="8">
+        <v>1045012304</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>54</v>
@@ -1219,8 +1219,8 @@
       <c r="T10" s="17"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
-        <v>8</v>
+      <c r="B11" s="8">
+        <v>1045012308</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -1234,8 +1234,8 @@
       <c r="G11" s="3">
         <v>8</v>
       </c>
-      <c r="H11" s="2">
-        <v>4</v>
+      <c r="H11" s="8">
+        <v>1045012304</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>55</v>
@@ -1255,8 +1255,8 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <v>9</v>
+      <c r="B12" s="8">
+        <v>1045012309</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -1270,8 +1270,8 @@
       <c r="G12" s="3">
         <v>9</v>
       </c>
-      <c r="H12" s="2">
-        <v>5</v>
+      <c r="H12" s="8">
+        <v>1045012305</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>56</v>
@@ -1291,8 +1291,8 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <v>10</v>
+      <c r="B13" s="8">
+        <v>1045012310</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
@@ -1306,8 +1306,8 @@
       <c r="G13" s="3">
         <v>10</v>
       </c>
-      <c r="H13" s="2">
-        <v>5</v>
+      <c r="H13" s="8">
+        <v>1045012305</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>57</v>
@@ -1327,8 +1327,8 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <v>11</v>
+      <c r="B14" s="8">
+        <v>1045012311</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
@@ -1342,8 +1342,8 @@
       <c r="G14" s="3">
         <v>11</v>
       </c>
-      <c r="H14" s="2">
-        <v>6</v>
+      <c r="H14" s="8">
+        <v>1045012306</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>58</v>
@@ -1363,8 +1363,8 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
-        <v>12</v>
+      <c r="B15" s="8">
+        <v>1045012312</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -1378,8 +1378,8 @@
       <c r="G15" s="3">
         <v>12</v>
       </c>
-      <c r="H15" s="2">
-        <v>6</v>
+      <c r="H15" s="8">
+        <v>1045012306</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>48</v>
@@ -1399,8 +1399,8 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
-        <v>13</v>
+      <c r="B16" s="8">
+        <v>1045012313</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -1414,8 +1414,8 @@
       <c r="G16" s="3">
         <v>13</v>
       </c>
-      <c r="H16" s="2">
-        <v>7</v>
+      <c r="H16" s="8">
+        <v>1045012307</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>49</v>
@@ -1435,8 +1435,8 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
-        <v>14</v>
+      <c r="B17" s="8">
+        <v>1045012314</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
@@ -1450,8 +1450,8 @@
       <c r="G17" s="3">
         <v>14</v>
       </c>
-      <c r="H17" s="2">
-        <v>7</v>
+      <c r="H17" s="8">
+        <v>1045012307</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>50</v>
@@ -1471,8 +1471,8 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="3">
-        <v>15</v>
+      <c r="B18" s="8">
+        <v>1045012315</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -1486,8 +1486,8 @@
       <c r="G18" s="3">
         <v>15</v>
       </c>
-      <c r="H18" s="2">
-        <v>8</v>
+      <c r="H18" s="8">
+        <v>1045012308</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>51</v>
@@ -1507,8 +1507,8 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="3">
-        <v>16</v>
+      <c r="B19" s="8">
+        <v>1045012316</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
@@ -1522,8 +1522,8 @@
       <c r="G19" s="3">
         <v>16</v>
       </c>
-      <c r="H19" s="2">
-        <v>8</v>
+      <c r="H19" s="8">
+        <v>1045012308</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>52</v>
@@ -1543,8 +1543,8 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="3">
-        <v>17</v>
+      <c r="B20" s="8">
+        <v>1045012317</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>20</v>
@@ -1558,8 +1558,8 @@
       <c r="G20" s="3">
         <v>17</v>
       </c>
-      <c r="H20" s="2">
-        <v>9</v>
+      <c r="H20" s="8">
+        <v>1045012309</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>53</v>
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
-        <v>18</v>
+      <c r="B21" s="8">
+        <v>1045012318</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
@@ -1594,8 +1594,8 @@
       <c r="G21" s="3">
         <v>18</v>
       </c>
-      <c r="H21" s="2">
-        <v>9</v>
+      <c r="H21" s="8">
+        <v>1045012309</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>54</v>
@@ -1615,8 +1615,8 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="3">
-        <v>19</v>
+      <c r="B22" s="8">
+        <v>1045012319</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
@@ -1630,8 +1630,8 @@
       <c r="G22" s="3">
         <v>19</v>
       </c>
-      <c r="H22" s="2">
-        <v>10</v>
+      <c r="H22" s="8">
+        <v>1045012310</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>55</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5">
-        <v>20</v>
+        <v>1045012320</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>23</v>
@@ -1666,8 +1666,8 @@
       <c r="G23" s="3">
         <v>20</v>
       </c>
-      <c r="H23" s="2">
-        <v>10</v>
+      <c r="H23" s="8">
+        <v>1045012310</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>56</v>
@@ -1690,8 +1690,8 @@
       <c r="G24" s="3">
         <v>21</v>
       </c>
-      <c r="H24" s="2">
-        <v>11</v>
+      <c r="H24" s="8">
+        <v>1045012311</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>57</v>
@@ -1714,8 +1714,8 @@
       <c r="G25" s="3">
         <v>22</v>
       </c>
-      <c r="H25" s="2">
-        <v>11</v>
+      <c r="H25" s="8">
+        <v>1045012311</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>58</v>
@@ -1738,8 +1738,8 @@
       <c r="G26" s="3">
         <v>23</v>
       </c>
-      <c r="H26" s="2">
-        <v>12</v>
+      <c r="H26" s="8">
+        <v>1045012312</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>48</v>
@@ -1762,8 +1762,8 @@
       <c r="G27" s="3">
         <v>24</v>
       </c>
-      <c r="H27" s="2">
-        <v>12</v>
+      <c r="H27" s="8">
+        <v>1045012312</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>49</v>
@@ -1786,8 +1786,8 @@
       <c r="G28" s="3">
         <v>25</v>
       </c>
-      <c r="H28" s="2">
-        <v>13</v>
+      <c r="H28" s="8">
+        <v>1045012313</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>50</v>
@@ -1810,8 +1810,8 @@
       <c r="G29" s="3">
         <v>26</v>
       </c>
-      <c r="H29" s="2">
-        <v>13</v>
+      <c r="H29" s="8">
+        <v>1045012313</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>51</v>
@@ -1834,8 +1834,8 @@
       <c r="G30" s="3">
         <v>27</v>
       </c>
-      <c r="H30" s="2">
-        <v>14</v>
+      <c r="H30" s="8">
+        <v>1045012314</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>52</v>
@@ -1858,8 +1858,8 @@
       <c r="G31" s="3">
         <v>28</v>
       </c>
-      <c r="H31" s="2">
-        <v>14</v>
+      <c r="H31" s="8">
+        <v>1045012314</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>53</v>
@@ -1882,8 +1882,8 @@
       <c r="G32" s="3">
         <v>29</v>
       </c>
-      <c r="H32" s="2">
-        <v>15</v>
+      <c r="H32" s="8">
+        <v>1045012315</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>54</v>
@@ -1906,8 +1906,8 @@
       <c r="G33" s="3">
         <v>30</v>
       </c>
-      <c r="H33" s="2">
-        <v>15</v>
+      <c r="H33" s="8">
+        <v>1045012315</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>55</v>
@@ -1930,8 +1930,8 @@
       <c r="G34" s="3">
         <v>31</v>
       </c>
-      <c r="H34" s="2">
-        <v>16</v>
+      <c r="H34" s="8">
+        <v>1045012316</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>56</v>
@@ -1954,8 +1954,8 @@
       <c r="G35" s="3">
         <v>32</v>
       </c>
-      <c r="H35" s="2">
-        <v>16</v>
+      <c r="H35" s="8">
+        <v>1045012316</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>57</v>
@@ -1978,8 +1978,8 @@
       <c r="G36" s="3">
         <v>33</v>
       </c>
-      <c r="H36" s="2">
-        <v>17</v>
+      <c r="H36" s="8">
+        <v>1045012317</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>58</v>
@@ -2002,8 +2002,8 @@
       <c r="G37" s="3">
         <v>34</v>
       </c>
-      <c r="H37" s="2">
-        <v>17</v>
+      <c r="H37" s="8">
+        <v>1045012317</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>48</v>
@@ -2026,8 +2026,8 @@
       <c r="G38" s="3">
         <v>35</v>
       </c>
-      <c r="H38" s="2">
-        <v>18</v>
+      <c r="H38" s="8">
+        <v>1045012318</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>49</v>
@@ -2050,8 +2050,8 @@
       <c r="G39" s="3">
         <v>36</v>
       </c>
-      <c r="H39" s="2">
-        <v>18</v>
+      <c r="H39" s="8">
+        <v>1045012318</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>50</v>
@@ -2074,8 +2074,8 @@
       <c r="G40" s="3">
         <v>37</v>
       </c>
-      <c r="H40" s="2">
-        <v>19</v>
+      <c r="H40" s="8">
+        <v>1045012319</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>51</v>
@@ -2098,8 +2098,8 @@
       <c r="G41" s="3">
         <v>38</v>
       </c>
-      <c r="H41" s="2">
-        <v>19</v>
+      <c r="H41" s="8">
+        <v>1045012319</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>52</v>
@@ -2122,8 +2122,8 @@
       <c r="G42" s="3">
         <v>39</v>
       </c>
-      <c r="H42" s="2">
-        <v>20</v>
+      <c r="H42" s="8">
+        <v>1045012320</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>59</v>
@@ -2146,8 +2146,8 @@
       <c r="G43" s="3">
         <v>40</v>
       </c>
-      <c r="H43" s="2">
-        <v>20</v>
+      <c r="H43" s="8">
+        <v>1045012320</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>54</v>
@@ -2170,8 +2170,8 @@
       <c r="G44" s="3">
         <v>41</v>
       </c>
-      <c r="H44" s="2">
-        <v>1</v>
+      <c r="H44" s="8">
+        <v>1045012301</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>55</v>
@@ -2194,8 +2194,8 @@
       <c r="G45" s="3">
         <v>42</v>
       </c>
-      <c r="H45" s="2">
-        <v>2</v>
+      <c r="H45" s="8">
+        <v>1045012302</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>56</v>
@@ -2218,8 +2218,8 @@
       <c r="G46" s="3">
         <v>43</v>
       </c>
-      <c r="H46" s="2">
-        <v>3</v>
+      <c r="H46" s="8">
+        <v>1045012303</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>57</v>
@@ -2242,8 +2242,8 @@
       <c r="G47" s="3">
         <v>44</v>
       </c>
-      <c r="H47" s="2">
-        <v>4</v>
+      <c r="H47" s="8">
+        <v>1045012304</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>58</v>
@@ -2266,8 +2266,8 @@
       <c r="G48" s="3">
         <v>45</v>
       </c>
-      <c r="H48" s="2">
-        <v>5</v>
+      <c r="H48" s="8">
+        <v>1045012305</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>48</v>
@@ -2290,8 +2290,8 @@
       <c r="G49" s="3">
         <v>46</v>
       </c>
-      <c r="H49" s="2">
-        <v>6</v>
+      <c r="H49" s="8">
+        <v>1045012306</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>49</v>
@@ -2314,8 +2314,8 @@
       <c r="G50" s="3">
         <v>47</v>
       </c>
-      <c r="H50" s="2">
-        <v>7</v>
+      <c r="H50" s="8">
+        <v>1045012307</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>50</v>
@@ -2338,8 +2338,8 @@
       <c r="G51" s="3">
         <v>48</v>
       </c>
-      <c r="H51" s="2">
-        <v>8</v>
+      <c r="H51" s="8">
+        <v>1045012308</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>60</v>
@@ -2362,8 +2362,8 @@
       <c r="G52" s="3">
         <v>49</v>
       </c>
-      <c r="H52" s="2">
-        <v>9</v>
+      <c r="H52" s="8">
+        <v>1045012309</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>52</v>
@@ -2386,8 +2386,8 @@
       <c r="G53" s="5">
         <v>50</v>
       </c>
-      <c r="H53" s="6">
-        <v>10</v>
+      <c r="H53" s="5">
+        <v>1045012310</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>61</v>

</xml_diff>